<commit_message>
2nd week intermediate 1 updates
</commit_message>
<xml_diff>
--- a/Excel Intermediate Skills I/Week 2/Test your Skills/C2 W2 Assessment Workbook.xlsx
+++ b/Excel Intermediate Skills I/Week 2/Test your Skills/C2 W2 Assessment Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohamed/Desktop/Directories/Excel Exercises/Excel Intermediate Skills I/Week 2/Test your Skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10E0B1E-3DAA-A64F-A243-BB400EAB674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA72311-729E-4242-8930-29A7BC0B89D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="13840" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -37,28 +37,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -966,7 +944,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2138,10 +2116,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2153,14 +2131,15 @@
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="6.1640625" customWidth="1"/>
     <col min="7" max="8" width="6.83203125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="26.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
@@ -2181,267 +2160,745 @@
       </c>
       <c r="H4" s="21"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="e" cm="1">
-        <f t="array" ref="A5">SKU&amp;Inventory!D4&amp;"-"&amp;Inventory!A4</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D4&amp;"-"&amp;Inventory!A4</f>
+        <v>SKU-07-2425</v>
+      </c>
+      <c r="B5" s="18" t="str">
+        <f>UPPER(Inventory!C4)</f>
+        <v>GLASS</v>
+      </c>
+      <c r="C5" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E4,5))</f>
+        <v>dynam</v>
+      </c>
+      <c r="D5" s="19" t="str">
+        <f>LEFT(Inventory!B4,FIND(",",Inventory!B4)-1)</f>
+        <v>Solar Glass (Low Iron Tempered)</v>
+      </c>
+      <c r="E5" s="19" t="str">
+        <f>RIGHT(Inventory!F4,3)&amp;MID(Inventory!F4,FIND(",",Inventory!F4)+2,4)</f>
+        <v>NSW2007</v>
+      </c>
       <c r="G5" s="17">
         <v>1</v>
       </c>
       <c r="H5" s="17">
         <f t="array" aca="1" ref="H5:H9" ca="1">TRANSPOSE('Check Digit'!B23:F23)</f>
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D5&amp;"-"&amp;Inventory!A5</f>
+        <v>SKU-01-2213</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>UPPER(Inventory!C5)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C6" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E5,5))</f>
+        <v>metal</v>
+      </c>
+      <c r="D6" s="19" t="str">
+        <f>LEFT(Inventory!B5,FIND(",",Inventory!B5)-1)</f>
+        <v>Aluminum 6061-T6 Bare Sheet</v>
+      </c>
+      <c r="E6" s="19" t="str">
+        <f>RIGHT(Inventory!F5,3)&amp;MID(Inventory!F5,FIND(",",Inventory!F5)+2,4)</f>
+        <v>VIC3182</v>
+      </c>
       <c r="G6" s="17">
         <v>2</v>
       </c>
       <c r="H6" s="17">
         <f ca="1"/>
-        <v>5852</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+        <v>5827</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D6&amp;"-"&amp;Inventory!A6</f>
+        <v>SKU-12-2381</v>
+      </c>
+      <c r="B7" s="18" t="str">
+        <f>UPPER(Inventory!C6)</f>
+        <v>POLYCARBONATE</v>
+      </c>
+      <c r="C7" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E6,5))</f>
+        <v>harri</v>
+      </c>
+      <c r="D7" s="19" t="str">
+        <f>LEFT(Inventory!B6,FIND(",",Inventory!B6)-1)</f>
+        <v>LEXAN Polycarbonate Sheet</v>
+      </c>
+      <c r="E7" s="19" t="str">
+        <f>RIGHT(Inventory!F6,3)&amp;MID(Inventory!F6,FIND(",",Inventory!F6)+2,4)</f>
+        <v>NSW2010</v>
+      </c>
       <c r="G7" s="17">
         <v>3</v>
       </c>
       <c r="H7" s="17">
         <f ca="1"/>
-        <v>7491</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+        <v>6275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D7&amp;"-"&amp;Inventory!A7</f>
+        <v>SKU-15-2097</v>
+      </c>
+      <c r="B8" s="18" t="str">
+        <f>UPPER(Inventory!C7)</f>
+        <v>RUBBER</v>
+      </c>
+      <c r="C8" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E7,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D8" s="19" t="str">
+        <f>LEFT(Inventory!B7,FIND(",",Inventory!B7)-1)</f>
+        <v>Washer</v>
+      </c>
+      <c r="E8" s="19" t="str">
+        <f>RIGHT(Inventory!F7,3)&amp;MID(Inventory!F7,FIND(",",Inventory!F7)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
       <c r="G8" s="17">
         <v>4</v>
       </c>
       <c r="H8" s="17">
         <f ca="1"/>
-        <v>5800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D8&amp;"-"&amp;Inventory!A8</f>
+        <v>SKU-17-2073</v>
+      </c>
+      <c r="B9" s="18" t="str">
+        <f>UPPER(Inventory!C8)</f>
+        <v>SILICON</v>
+      </c>
+      <c r="C9" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E8,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D9" s="19" t="str">
+        <f>LEFT(Inventory!B8,FIND(",",Inventory!B8)-1)</f>
+        <v>Sealant/Caulking</v>
+      </c>
+      <c r="E9" s="19" t="str">
+        <f>RIGHT(Inventory!F8,3)&amp;MID(Inventory!F8,FIND(",",Inventory!F8)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
       <c r="G9" s="17">
         <v>5</v>
       </c>
       <c r="H9" s="17">
         <f ca="1"/>
-        <v>5247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+        <v>7022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D9&amp;"-"&amp;Inventory!A9</f>
+        <v>SKU-01-2290</v>
+      </c>
+      <c r="B10" s="18" t="str">
+        <f>UPPER(Inventory!C9)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C10" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E9,5))</f>
+        <v>metal</v>
+      </c>
+      <c r="D10" s="19" t="str">
+        <f>LEFT(Inventory!B9,FIND(",",Inventory!B9)-1)</f>
+        <v>Aluminum 6061-T6</v>
+      </c>
+      <c r="E10" s="19" t="str">
+        <f>RIGHT(Inventory!F9,3)&amp;MID(Inventory!F9,FIND(",",Inventory!F9)+2,4)</f>
+        <v>VIC3182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D10&amp;"-"&amp;Inventory!A10</f>
+        <v>SKU-11-2850</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>UPPER(Inventory!C10)</f>
+        <v>PLASTIC</v>
+      </c>
+      <c r="C11" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E10,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D11" s="19" t="str">
+        <f>LEFT(Inventory!B10,FIND(",",Inventory!B10)-1)</f>
+        <v>Quick-Disconnect Tube Couplings</v>
+      </c>
+      <c r="E11" s="19" t="str">
+        <f>RIGHT(Inventory!F10,3)&amp;MID(Inventory!F10,FIND(",",Inventory!F10)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D11&amp;"-"&amp;Inventory!A11</f>
+        <v>SKU-11-2369</v>
+      </c>
+      <c r="B12" s="18" t="str">
+        <f>UPPER(Inventory!C11)</f>
+        <v>PLASTIC</v>
+      </c>
+      <c r="C12" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E11,5))</f>
+        <v>fresh</v>
+      </c>
+      <c r="D12" s="19" t="str">
+        <f>LEFT(Inventory!B11,FIND(",",Inventory!B11)-1)</f>
+        <v>Mini Adjustable Float Valve</v>
+      </c>
+      <c r="E12" s="19" t="str">
+        <f>RIGHT(Inventory!F11,3)&amp;MID(Inventory!F11,FIND(",",Inventory!F11)+2,4)</f>
+        <v>VIC3121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D12&amp;"-"&amp;Inventory!A12</f>
+        <v>SKU-13-2082</v>
+      </c>
+      <c r="B13" s="18" t="str">
+        <f>UPPER(Inventory!C12)</f>
+        <v>POLYETHYLENE</v>
+      </c>
+      <c r="C13" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E12,5))</f>
+        <v xml:space="preserve">foam </v>
+      </c>
+      <c r="D13" s="19" t="str">
+        <f>LEFT(Inventory!B12,FIND(",",Inventory!B12)-1)</f>
+        <v>Closed Cell Foam</v>
+      </c>
+      <c r="E13" s="19" t="str">
+        <f>RIGHT(Inventory!F12,3)&amp;MID(Inventory!F12,FIND(",",Inventory!F12)+2,4)</f>
+        <v>NSW2018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D13&amp;"-"&amp;Inventory!A13</f>
+        <v>SKU-19-2485</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>UPPER(Inventory!C13)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C14" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E13,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D14" s="19" t="str">
+        <f>LEFT(Inventory!B13,FIND(",",Inventory!B13)-1)</f>
+        <v>Draw Latches</v>
+      </c>
+      <c r="E14" s="19" t="str">
+        <f>RIGHT(Inventory!F13,3)&amp;MID(Inventory!F13,FIND(",",Inventory!F13)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D14&amp;"-"&amp;Inventory!A14</f>
+        <v>SKU-16-2900</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>UPPER(Inventory!C14)</f>
+        <v>SALT</v>
+      </c>
+      <c r="C15" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E14,5))</f>
+        <v>aquar</v>
+      </c>
+      <c r="D15" s="19" t="str">
+        <f>LEFT(Inventory!B14,FIND(",",Inventory!B14)-1)</f>
+        <v>Tropic Marin Sea Salt</v>
+      </c>
+      <c r="E15" s="19" t="str">
+        <f>RIGHT(Inventory!F14,3)&amp;MID(Inventory!F14,FIND(",",Inventory!F14)+2,4)</f>
+        <v>VIC3181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D15&amp;"-"&amp;Inventory!A15</f>
+        <v>SKU-19-2255</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>UPPER(Inventory!C15)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C16" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E15,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D16" s="19" t="str">
+        <f>LEFT(Inventory!B15,FIND(",",Inventory!B15)-1)</f>
+        <v>Cap Screws</v>
+      </c>
+      <c r="E16" s="19" t="str">
+        <f>RIGHT(Inventory!F15,3)&amp;MID(Inventory!F15,FIND(",",Inventory!F15)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="A17" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D16&amp;"-"&amp;Inventory!A16</f>
+        <v>SKU-19-2568</v>
+      </c>
+      <c r="B17" s="18" t="str">
+        <f>UPPER(Inventory!C16)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C17" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E16,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D17" s="19" t="str">
+        <f>LEFT(Inventory!B16,FIND(",",Inventory!B16)-1)</f>
+        <v>Cap Screws</v>
+      </c>
+      <c r="E17" s="19" t="str">
+        <f>RIGHT(Inventory!F16,3)&amp;MID(Inventory!F16,FIND(",",Inventory!F16)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="A18" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D17&amp;"-"&amp;Inventory!A17</f>
+        <v>SKU-19-2676</v>
+      </c>
+      <c r="B18" s="18" t="str">
+        <f>UPPER(Inventory!C17)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C18" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E17,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D18" s="19" t="str">
+        <f>LEFT(Inventory!B17,FIND(",",Inventory!B17)-1)</f>
+        <v>Cap Screws</v>
+      </c>
+      <c r="E18" s="19" t="str">
+        <f>RIGHT(Inventory!F17,3)&amp;MID(Inventory!F17,FIND(",",Inventory!F17)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="A19" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D18&amp;"-"&amp;Inventory!A18</f>
+        <v>SKU-15-2658</v>
+      </c>
+      <c r="B19" s="18" t="str">
+        <f>UPPER(Inventory!C18)</f>
+        <v>RUBBER</v>
+      </c>
+      <c r="C19" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E18,5))</f>
+        <v>garlo</v>
+      </c>
+      <c r="D19" s="19" t="str">
+        <f>LEFT(Inventory!B18,FIND(",",Inventory!B18)-1)</f>
+        <v>Red SBR Rubber Sheet (Custom Cut Gasket)</v>
+      </c>
+      <c r="E19" s="19" t="str">
+        <f>RIGHT(Inventory!F18,3)&amp;MID(Inventory!F18,FIND(",",Inventory!F18)+2,4)</f>
+        <v>NSW2135</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="A20" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D19&amp;"-"&amp;Inventory!A19</f>
+        <v>SKU-09-2350</v>
+      </c>
+      <c r="B20" s="18" t="str">
+        <f>UPPER(Inventory!C19)</f>
+        <v>PAINT</v>
+      </c>
+      <c r="C20" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E19,5))</f>
+        <v>harri</v>
+      </c>
+      <c r="D20" s="19" t="str">
+        <f>LEFT(Inventory!B19,FIND(",",Inventory!B19)-1)</f>
+        <v>Rust-Oleum</v>
+      </c>
+      <c r="E20" s="19" t="str">
+        <f>RIGHT(Inventory!F19,3)&amp;MID(Inventory!F19,FIND(",",Inventory!F19)+2,4)</f>
+        <v>NSW2010</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="A21" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D20&amp;"-"&amp;Inventory!A20</f>
+        <v>SKU-11-2252</v>
+      </c>
+      <c r="B21" s="18" t="str">
+        <f>UPPER(Inventory!C20)</f>
+        <v>PLASTIC</v>
+      </c>
+      <c r="C21" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E20,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D21" s="19" t="str">
+        <f>LEFT(Inventory!B20,FIND(",",Inventory!B20)-1)</f>
+        <v>Containment Unit</v>
+      </c>
+      <c r="E21" s="19" t="str">
+        <f>RIGHT(Inventory!F20,3)&amp;MID(Inventory!F20,FIND(",",Inventory!F20)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="A22" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D21&amp;"-"&amp;Inventory!A21</f>
+        <v>SKU-08-2937</v>
+      </c>
+      <c r="B22" s="18" t="str">
+        <f>UPPER(Inventory!C21)</f>
+        <v>OSB</v>
+      </c>
+      <c r="C22" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E21,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D22" s="19" t="str">
+        <f>LEFT(Inventory!B21,FIND(",",Inventory!B21)-1)</f>
+        <v>Backboard</v>
+      </c>
+      <c r="E22" s="19" t="str">
+        <f>RIGHT(Inventory!F21,3)&amp;MID(Inventory!F21,FIND(",",Inventory!F21)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
+      <c r="A23" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D22&amp;"-"&amp;Inventory!A22</f>
+        <v>SKU-10-2553</v>
+      </c>
+      <c r="B23" s="18" t="str">
+        <f>UPPER(Inventory!C22)</f>
+        <v>PE</v>
+      </c>
+      <c r="C23" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E22,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D23" s="19" t="str">
+        <f>LEFT(Inventory!B22,FIND(",",Inventory!B22)-1)</f>
+        <v>Foam Board Insulation LD</v>
+      </c>
+      <c r="E23" s="19" t="str">
+        <f>RIGHT(Inventory!F22,3)&amp;MID(Inventory!F22,FIND(",",Inventory!F22)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="A24" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D23&amp;"-"&amp;Inventory!A23</f>
+        <v>SKU-02-2236</v>
+      </c>
+      <c r="B24" s="18" t="str">
+        <f>UPPER(Inventory!C23)</f>
+        <v>ACRYLIC</v>
+      </c>
+      <c r="C24" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E23,5))</f>
+        <v>roche</v>
+      </c>
+      <c r="D24" s="19" t="str">
+        <f>LEFT(Inventory!B23,FIND(",",Inventory!B23)-1)</f>
+        <v>Brackets</v>
+      </c>
+      <c r="E24" s="19" t="str">
+        <f>RIGHT(Inventory!F23,3)&amp;MID(Inventory!F23,FIND(",",Inventory!F23)+2,4)</f>
+        <v>NSW2204</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
+      <c r="A25" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D24&amp;"-"&amp;Inventory!A24</f>
+        <v>SKU-01-2785</v>
+      </c>
+      <c r="B25" s="18" t="str">
+        <f>UPPER(Inventory!C24)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C25" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E24,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D25" s="19" t="str">
+        <f>LEFT(Inventory!B24,FIND(",",Inventory!B24)-1)</f>
+        <v>Reflective Trough</v>
+      </c>
+      <c r="E25" s="19" t="str">
+        <f>RIGHT(Inventory!F24,3)&amp;MID(Inventory!F24,FIND(",",Inventory!F24)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
+      <c r="A26" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D25&amp;"-"&amp;Inventory!A25</f>
+        <v>SKU-04-2872</v>
+      </c>
+      <c r="B26" s="18" t="str">
+        <f>UPPER(Inventory!C25)</f>
+        <v>COPPER</v>
+      </c>
+      <c r="C26" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E25,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D26" s="19" t="str">
+        <f>LEFT(Inventory!B25,FIND(",",Inventory!B25)-1)</f>
+        <v>Receiver Pipe</v>
+      </c>
+      <c r="E26" s="19" t="str">
+        <f>RIGHT(Inventory!F25,3)&amp;MID(Inventory!F25,FIND(",",Inventory!F25)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
+      <c r="A27" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D26&amp;"-"&amp;Inventory!A26</f>
+        <v>SKU-14-2422</v>
+      </c>
+      <c r="B27" s="18" t="str">
+        <f>UPPER(Inventory!C26)</f>
+        <v>PVC</v>
+      </c>
+      <c r="C27" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E26,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D27" s="19" t="str">
+        <f>LEFT(Inventory!B26,FIND(",",Inventory!B26)-1)</f>
+        <v>PVC Pipe</v>
+      </c>
+      <c r="E27" s="19" t="str">
+        <f>RIGHT(Inventory!F26,3)&amp;MID(Inventory!F26,FIND(",",Inventory!F26)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
+      <c r="A28" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D27&amp;"-"&amp;Inventory!A27</f>
+        <v>SKU-14-2224</v>
+      </c>
+      <c r="B28" s="18" t="str">
+        <f>UPPER(Inventory!C27)</f>
+        <v>PVC</v>
+      </c>
+      <c r="C28" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E27,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D28" s="19" t="str">
+        <f>LEFT(Inventory!B27,FIND(",",Inventory!B27)-1)</f>
+        <v>PVC Fittings</v>
+      </c>
+      <c r="E28" s="19" t="str">
+        <f>RIGHT(Inventory!F27,3)&amp;MID(Inventory!F27,FIND(",",Inventory!F27)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
+      <c r="A29" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D28&amp;"-"&amp;Inventory!A28</f>
+        <v>SKU-10-2907</v>
+      </c>
+      <c r="B29" s="18" t="str">
+        <f>UPPER(Inventory!C28)</f>
+        <v>PE</v>
+      </c>
+      <c r="C29" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E28,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D29" s="19" t="str">
+        <f>LEFT(Inventory!B28,FIND(",",Inventory!B28)-1)</f>
+        <v>Pipe Insulation LD</v>
+      </c>
+      <c r="E29" s="19" t="str">
+        <f>RIGHT(Inventory!F28,3)&amp;MID(Inventory!F28,FIND(",",Inventory!F28)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="A30" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D29&amp;"-"&amp;Inventory!A29</f>
+        <v>SKU-18-2933</v>
+      </c>
+      <c r="B30" s="18" t="str">
+        <f>UPPER(Inventory!C29)</f>
+        <v>STAINLESS STEEL</v>
+      </c>
+      <c r="C30" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E29,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D30" s="19" t="str">
+        <f>LEFT(Inventory!B29,FIND(",",Inventory!B29)-1)</f>
+        <v>Housing Case</v>
+      </c>
+      <c r="E30" s="19" t="str">
+        <f>RIGHT(Inventory!F29,3)&amp;MID(Inventory!F29,FIND(",",Inventory!F29)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
+      <c r="A31" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D30&amp;"-"&amp;Inventory!A30</f>
+        <v>SKU-05-2133</v>
+      </c>
+      <c r="B31" s="18" t="str">
+        <f>UPPER(Inventory!C30)</f>
+        <v>FIBERGLASS</v>
+      </c>
+      <c r="C31" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E30,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D31" s="19" t="str">
+        <f>LEFT(Inventory!B30,FIND(",",Inventory!B30)-1)</f>
+        <v>Collector Back Insulation</v>
+      </c>
+      <c r="E31" s="19" t="str">
+        <f>RIGHT(Inventory!F30,3)&amp;MID(Inventory!F30,FIND(",",Inventory!F30)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
+      <c r="A32" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D31&amp;"-"&amp;Inventory!A31</f>
+        <v>SKU-04-2675</v>
+      </c>
+      <c r="B32" s="18" t="str">
+        <f>UPPER(Inventory!C31)</f>
+        <v>COPPER</v>
+      </c>
+      <c r="C32" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E31,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D32" s="19" t="str">
+        <f>LEFT(Inventory!B31,FIND(",",Inventory!B31)-1)</f>
+        <v>Receiver Tube</v>
+      </c>
+      <c r="E32" s="19" t="str">
+        <f>RIGHT(Inventory!F31,3)&amp;MID(Inventory!F31,FIND(",",Inventory!F31)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
+      <c r="A33" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D32&amp;"-"&amp;Inventory!A32</f>
+        <v>SKU-01-2932</v>
+      </c>
+      <c r="B33" s="18" t="str">
+        <f>UPPER(Inventory!C32)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C33" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E32,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D33" s="19" t="str">
+        <f>LEFT(Inventory!B32,FIND(",",Inventory!B32)-1)</f>
+        <v>Absorber Fins</v>
+      </c>
+      <c r="E33" s="19" t="str">
+        <f>RIGHT(Inventory!F32,3)&amp;MID(Inventory!F32,FIND(",",Inventory!F32)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
+      <c r="A34" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D33&amp;"-"&amp;Inventory!A33</f>
+        <v>SKU-06-2452</v>
+      </c>
+      <c r="B34" s="18" t="str">
+        <f>UPPER(Inventory!C33)</f>
+        <v>FOAM</v>
+      </c>
+      <c r="C34" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E33,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D34" s="19" t="str">
+        <f>LEFT(Inventory!B33,FIND(",",Inventory!B33)-1)</f>
+        <v>Pipe Insulation</v>
+      </c>
+      <c r="E34" s="19" t="str">
+        <f>RIGHT(Inventory!F33,3)&amp;MID(Inventory!F33,FIND(",",Inventory!F33)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
+      <c r="A35" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D34&amp;"-"&amp;Inventory!A34</f>
+        <v>SKU-06-2035</v>
+      </c>
+      <c r="B35" s="18" t="str">
+        <f>UPPER(Inventory!C34)</f>
+        <v>FOAM</v>
+      </c>
+      <c r="C35" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E34,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D35" s="19" t="str">
+        <f>LEFT(Inventory!B34,FIND(",",Inventory!B34)-1)</f>
+        <v>Pipe Insulation</v>
+      </c>
+      <c r="E35" s="19" t="str">
+        <f>RIGHT(Inventory!F34,3)&amp;MID(Inventory!F34,FIND(",",Inventory!F34)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
+      <c r="A36" s="18" t="str">
+        <f>"SKU-"&amp;Inventory!D35&amp;"-"&amp;Inventory!A35</f>
+        <v>SKU-17-2288</v>
+      </c>
+      <c r="B36" s="18" t="str">
+        <f>UPPER(Inventory!C35)</f>
+        <v>SILICON</v>
+      </c>
+      <c r="C36" s="18" t="str">
+        <f>LOWER(LEFT(Inventory!E35,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D36" s="19" t="str">
+        <f>LEFT(Inventory!B35,FIND(",",Inventory!B35)-1)</f>
+        <v>Sealant/Caulking</v>
+      </c>
+      <c r="E36" s="19" t="str">
+        <f>RIGHT(Inventory!F35,3)&amp;MID(Inventory!F35,FIND(",",Inventory!F35)+2,4)</f>
+        <v>NSW2000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2843,23 +3300,23 @@
       </c>
       <c r="B23" s="16">
         <f ca="1">IF(AND(B25,EXACT('For Printing'!A8,A8)),B18,IF(B25,B19,IF('For Printing'!A8="",B20,B21)))</f>
-        <v>1299</v>
+        <v>1767</v>
       </c>
       <c r="C23" s="16">
         <f ca="1">IF(AND(C25,EXACT('For Printing'!B8,B8)),C18,IF(C25,C19,IF('For Printing'!B8="",C20,C21)))</f>
-        <v>5852</v>
+        <v>5827</v>
       </c>
       <c r="D23" s="16">
         <f ca="1">IF(AND(D25,EXACT('For Printing'!C8,C8)),D18,IF(D25,D19,IF('For Printing'!C8="",D20,D21)))</f>
-        <v>7491</v>
+        <v>6275</v>
       </c>
       <c r="E23" s="16">
         <f ca="1">IF(AND(E25,EXACT('For Printing'!D8,D8)),E18,IF(E25,E19,IF('For Printing'!D8="",E20,E21)))</f>
-        <v>5800</v>
+        <v>3203</v>
       </c>
       <c r="F23" s="16">
         <f ca="1">IF(AND(F25,EXACT('For Printing'!E8,E8)),F18,IF(F25,F19,IF('For Printing'!E8="",F20,F21)))</f>
-        <v>5247</v>
+        <v>7022</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -2868,23 +3325,23 @@
       </c>
       <c r="B25" s="16" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,B28,B27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="16" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,C28,C27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="16" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,D28,D27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="16" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,E28,E27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="16" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,F28,F27)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>119</v>
@@ -2936,23 +3393,23 @@
       </c>
       <c r="B28" s="16" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!A8),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="16" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!B8),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="16" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!C8),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="16" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!D8),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="16" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!E8),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2961,23 +3418,23 @@
       </c>
       <c r="B30" s="16" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!A8),CELL("prefix",'For Printing'!A8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!A8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="16" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!B8),CELL("prefix",'For Printing'!B8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!B8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="16" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!C8),CELL("prefix",'For Printing'!C8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!C8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="16" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!D8),CELL("prefix",'For Printing'!D8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!D8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="16" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!E8),CELL("prefix",'For Printing'!E8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!E8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>118</v>

</xml_diff>